<commit_message>
Added LUT for DAc
</commit_message>
<xml_diff>
--- a/PES sine plot.xlsx
+++ b/PES sine plot.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prayag/Documents/MCUXpressoIDE_11.0.1/workspace/PES Project 6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B54979C-5639-0D4F-BD86-D09EBCCCE229}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850088AE-76CB-B741-AFE5-1A6F869F6827}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="460" windowWidth="24680" windowHeight="15000" xr2:uid="{C7706A3D-BCBB-674C-92B3-CB16D3F61D8F}"/>
   </bookViews>
@@ -319,37 +319,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A55F-5742-8AB2-5D568148670F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$B$1:$B$50</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A55F-5742-8AB2-5D568148670F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -554,7 +523,448 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$1:$B$50</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2478</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2637</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2792</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2943</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3086</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3219</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3340</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3447</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3538</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3611</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3666</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3702</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3717</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3712</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3686</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3641</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3577</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3495</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3396</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3281</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3154</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3016</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2869</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2715</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2557</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2399</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2241</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2087</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1940</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1802</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1675</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1560</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1461</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1379</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1315</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1270</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1244</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1239</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1254</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1290</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1345</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1418</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1509</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1616</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1737</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1870</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2164</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2319</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2478</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5AAD-874C-8FC6-BF0D407154D6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="155634687"/>
+        <c:axId val="155659759"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="155634687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="155659759"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="155659759"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="155634687"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1110,6 +1520,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1143,6 +2069,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9837911-E92E-2741-BC35-E24DBCB6AF32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1448,262 +2410,412 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FD162D-1D82-0048-9293-993E19AFB247}">
-  <dimension ref="A1:A50"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" s="1">
+        <v>2637</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" s="1">
+        <v>2792</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" s="1">
+        <v>2943</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <v>3086</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>3219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>3340</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>3447</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>0.86</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>3538</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0.91</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>3611</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>0.96</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
+        <v>3666</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B12" s="1">
+        <v>3702</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B13" s="1">
+        <v>3717</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B14" s="1">
+        <v>3712</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B15" s="1">
+        <v>3686</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>0.94</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
+        <v>3641</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>0.89</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17" s="1">
+        <v>3577</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18" s="1">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>0.74</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19" s="1">
+        <v>3396</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20" s="1">
+        <v>3281</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21" s="1">
+        <v>3154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22" s="1">
+        <v>3016</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" s="1">
+        <v>2869</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24" s="1">
+        <v>2715</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25" s="1">
+        <v>2557</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>-0.06</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26" s="1">
+        <v>2399</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>-0.19</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27" s="1">
+        <v>2241</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>-0.32</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28" s="1">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>-0.43</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29" s="1">
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>-0.55000000000000004</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" s="1">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>-0.65</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31" s="1">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>-0.74</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" s="1">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>-0.82</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" s="1">
+        <v>1461</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>-0.89</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" s="1">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>-0.94</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35" s="1">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>-0.97</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36" s="1">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37" s="1">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B38" s="1">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>-0.99</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B39" s="1">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>-0.96</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B40" s="1">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>-0.91</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B41" s="1">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>-0.86</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B42" s="1">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>-0.78</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B43" s="1">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>-0.7</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B44" s="1">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>-0.6</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B45" s="1">
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>-0.49</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B46" s="1">
+        <v>1870</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>-0.38</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B47" s="1">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>-0.25</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B48" s="1">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>-0.13</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B49" s="1">
+        <v>2319</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>0</v>
+      </c>
+      <c r="B50" s="1">
+        <v>2478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>